<commit_message>
Start new Flask App
</commit_message>
<xml_diff>
--- a/Flashcard_App/Flashcards Questions & Answers.xlsx
+++ b/Flashcard_App/Flashcards Questions & Answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpradetto/Desktop/Projects/Flashcard_App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66C6511-75E0-364C-87D3-BFFE1446C08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1864F2-720C-6943-BD8B-38E22DBBA9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="4" xr2:uid="{3654C377-FF8F-474F-9085-8FA19E1F1447}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="5" xr2:uid="{3654C377-FF8F-474F-9085-8FA19E1F1447}"/>
   </bookViews>
   <sheets>
     <sheet name="LINKED_LISTS" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ARRAYS" sheetId="3" r:id="rId3"/>
     <sheet name="STACKS" sheetId="4" r:id="rId4"/>
     <sheet name="QUEUES" sheetId="5" r:id="rId5"/>
+    <sheet name="BIG O" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
   <si>
     <t>Flashcard Front</t>
   </si>
@@ -238,13 +239,94 @@
   </si>
   <si>
     <t>Constant O(1) - pop remove a person in queue but remember it comes from the front of the line</t>
+  </si>
+  <si>
+    <r>
+      <t>O(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> == "constant"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O(log n)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> == "logarithmic"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O(n)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> == "linear"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O(n^2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> == "quadratic"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O(n^3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> == "cubic"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O(2^n)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF232629"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> == "exponential"</t>
+    </r>
+  </si>
+  <si>
+    <t>O(n log n) == "linearithmic"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -254,6 +336,24 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF232629"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF232629"/>
+      <name val="Var(--ff-mono)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -276,16 +376,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,7 +708,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
@@ -612,7 +716,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="34">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -640,7 +744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="34">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -656,7 +760,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -664,7 +768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -672,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="68">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -680,7 +784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="34">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -702,7 +806,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
@@ -710,7 +814,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="34">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -738,7 +842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="34">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -746,7 +850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="34">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -754,7 +858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="34">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -762,7 +866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="51">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -770,7 +874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="34">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -791,7 +895,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
@@ -799,7 +903,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -827,7 +931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -835,7 +939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="34">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -843,7 +947,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -851,7 +955,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -859,7 +963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="68">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -867,7 +971,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="51">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -875,7 +979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="51">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -896,7 +1000,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
@@ -904,7 +1008,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,7 +1028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="34">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -932,7 +1036,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="34">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -940,7 +1044,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="34">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -948,7 +1052,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -956,7 +1060,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -964,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -972,7 +1076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="51">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
@@ -980,7 +1084,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -997,11 +1101,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E767B4-E6FA-8444-A1AE-81C3D8A703B9}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
+    <sheetView zoomScale="162" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
@@ -1009,7 +1113,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -1037,7 +1141,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="34">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1045,7 +1149,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="34">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -1053,7 +1157,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
@@ -1061,7 +1165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="51">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -1069,7 +1173,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -1077,7 +1181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="51">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
@@ -1085,7 +1189,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1096,4 +1200,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696A23F2-61F7-FF4B-BC25-A575C00B2455}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="19">
+      <c r="A1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="19">
+      <c r="A2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="19">
+      <c r="A3" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="19">
+      <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="19">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="19">
+      <c r="A6" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" location="Linearithmic.2Fquasilinear_time" display="http://en.wikipedia.org/wiki/Time_complexity - Linearithmic.2Fquasilinear_time" xr:uid="{B157CE0F-FD28-1847-ADE9-6ECEF04D98BB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>